<commit_message>
Update Leave Card 1/17/2024 3:57 pm
</commit_message>
<xml_diff>
--- a/CASUAL/LA SP-VMO/ANGELES, ANNABEL DIMARANAN.xlsx
+++ b/CASUAL/LA SP-VMO/ANGELES, ANNABEL DIMARANAN.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="111">
   <si>
     <t>PERIOD</t>
   </si>
@@ -342,61 +342,25 @@
     <t>UT(0-5-22)</t>
   </si>
   <si>
-    <t>A(3-0-0)</t>
-  </si>
-  <si>
-    <t>11/7,28,29/2022</t>
-  </si>
-  <si>
-    <t>A(1-0-0)</t>
-  </si>
-  <si>
     <t>UT(0-1-2)</t>
   </si>
   <si>
     <t>UT(0-3-56)</t>
   </si>
   <si>
-    <t>A(4-0-0)</t>
-  </si>
-  <si>
-    <t>8/8,11,15,19/2022</t>
-  </si>
-  <si>
     <t>UT(0-0-47)</t>
   </si>
   <si>
     <t>UT(0-1-41)</t>
   </si>
   <si>
-    <t>A(10-0-0)</t>
-  </si>
-  <si>
-    <t>6/1,2,9,10,14,17,20,22-24/2022</t>
-  </si>
-  <si>
     <t>UT(0-3-35)</t>
   </si>
   <si>
-    <t>A(14-0-0)</t>
-  </si>
-  <si>
-    <t>5/2,3,4,5,6,11,12,13,16,17,18,19,20/2022</t>
-  </si>
-  <si>
     <t>UT(0-0-24)</t>
   </si>
   <si>
-    <t>A(16-0-0)</t>
-  </si>
-  <si>
-    <t>4/4-8,11-13,18-21,26-29/2022</t>
-  </si>
-  <si>
     <t>UT(0-0-6)</t>
-  </si>
-  <si>
-    <t>3/11,21,23,24/2022</t>
   </si>
   <si>
     <t>UT(0-2-49)</t>
@@ -790,17 +754,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -810,6 +771,9 @@
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1340,7 +1304,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1383,7 +1347,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1447,7 +1411,7 @@
         <xdr:cNvPr id="4" name="Arrow: Left 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1507,7 +1471,7 @@
         <xdr:cNvPr id="8" name="Oval 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1573,7 +1537,7 @@
         <xdr:cNvPr id="9" name="Arrow: Left-Right 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1636,7 +1600,7 @@
         <xdr:cNvPr id="10" name="TextBox 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1734,7 +1698,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1793,7 +1757,7 @@
         <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1858,7 +1822,7 @@
         <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1901,7 +1865,7 @@
         <xdr:cNvPr id="21" name="TextBox 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1976,7 +1940,7 @@
         <xdr:cNvPr id="22" name="TextBox 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2162,7 +2126,7 @@
         <xdr:cNvPr id="23" name="Oval 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2228,7 +2192,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2286,7 +2250,7 @@
         <xdr:cNvPr id="26" name="Oval 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2352,7 +2316,7 @@
         <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2408,7 +2372,7 @@
         <xdr:cNvPr id="30" name="TextBox 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2483,7 +2447,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2526,7 +2490,7 @@
         <xdr:cNvPr id="32" name="Oval 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2592,7 +2556,7 @@
         <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2648,7 +2612,7 @@
         <xdr:cNvPr id="34" name="TextBox 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2744,7 +2708,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A8:K132" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A8:K125" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <tableColumns count="11">
     <tableColumn id="1" name="PERIOD" dataDxfId="25"/>
     <tableColumn id="2" name="PARTICULARS" dataDxfId="24"/>
@@ -3121,12 +3085,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:K132"/>
+  <dimension ref="A2:K125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3690" topLeftCell="A80" activePane="bottomLeft"/>
+      <pane ySplit="3690" topLeftCell="A59" activePane="bottomLeft"/>
       <selection activeCell="I10" sqref="I10"/>
-      <selection pane="bottomLeft" activeCell="D96" sqref="D96"/>
+      <selection pane="bottomLeft" activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3156,14 +3120,14 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="53"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -3174,16 +3138,16 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="55">
+      <c r="F3" s="54">
         <v>43101</v>
       </c>
-      <c r="G3" s="51"/>
+      <c r="G3" s="52"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="57"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="56"/>
     </row>
     <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
@@ -3196,16 +3160,16 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="51"/>
+      <c r="G4" s="52"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="53"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
@@ -3231,18 +3195,18 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53" t="s">
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
       <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -3289,7 +3253,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table13[EARNED])-SUM(Table13[Absence Undertime W/ Pay])</f>
-        <v>-1.4620000000000033</v>
+        <v>50.537999999999997</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -4419,13 +4383,13 @@
         <v>44621</v>
       </c>
       <c r="B65" s="20" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C65" s="13">
         <v>1.25</v>
       </c>
       <c r="D65" s="39">
-        <v>4</v>
+        <v>0.35199999999999998</v>
       </c>
       <c r="E65" s="9"/>
       <c r="F65" s="20"/>
@@ -4436,24 +4400,26 @@
       <c r="H65" s="39"/>
       <c r="I65" s="9"/>
       <c r="J65" s="11"/>
-      <c r="K65" s="20" t="s">
-        <v>119</v>
-      </c>
+      <c r="K65" s="20"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="40"/>
+      <c r="A66" s="40">
+        <v>44652</v>
+      </c>
       <c r="B66" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="C66" s="13"/>
+        <v>107</v>
+      </c>
+      <c r="C66" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D66" s="39">
-        <v>0.35199999999999998</v>
+        <v>1.2E-2</v>
       </c>
       <c r="E66" s="9"/>
       <c r="F66" s="20"/>
-      <c r="G66" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G66" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H66" s="39"/>
       <c r="I66" s="9"/>
@@ -4462,16 +4428,16 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="40">
-        <v>44652</v>
+        <v>44682</v>
       </c>
       <c r="B67" s="20" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C67" s="13">
         <v>1.25</v>
       </c>
       <c r="D67" s="39">
-        <v>16</v>
+        <v>5.000000000000001E-2</v>
       </c>
       <c r="E67" s="9"/>
       <c r="F67" s="20"/>
@@ -4482,24 +4448,26 @@
       <c r="H67" s="39"/>
       <c r="I67" s="9"/>
       <c r="J67" s="11"/>
-      <c r="K67" s="20" t="s">
-        <v>117</v>
-      </c>
+      <c r="K67" s="20"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="40"/>
+      <c r="A68" s="40">
+        <v>44713</v>
+      </c>
       <c r="B68" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="C68" s="13"/>
+        <v>105</v>
+      </c>
+      <c r="C68" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D68" s="39">
-        <v>1.2E-2</v>
+        <v>0.44800000000000001</v>
       </c>
       <c r="E68" s="9"/>
       <c r="F68" s="20"/>
-      <c r="G68" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G68" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H68" s="39"/>
       <c r="I68" s="9"/>
@@ -4508,16 +4476,16 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="40">
-        <v>44682</v>
+        <v>44743</v>
       </c>
       <c r="B69" s="20" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C69" s="13">
         <v>1.25</v>
       </c>
       <c r="D69" s="39">
-        <v>14</v>
+        <v>0.21000000000000002</v>
       </c>
       <c r="E69" s="9"/>
       <c r="F69" s="20"/>
@@ -4528,24 +4496,26 @@
       <c r="H69" s="39"/>
       <c r="I69" s="9"/>
       <c r="J69" s="11"/>
-      <c r="K69" s="20" t="s">
-        <v>114</v>
-      </c>
+      <c r="K69" s="20"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A70" s="40"/>
+      <c r="A70" s="40">
+        <v>44774</v>
+      </c>
       <c r="B70" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="C70" s="13"/>
+        <v>103</v>
+      </c>
+      <c r="C70" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D70" s="39">
-        <v>5.000000000000001E-2</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="E70" s="9"/>
       <c r="F70" s="20"/>
-      <c r="G70" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G70" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H70" s="39"/>
       <c r="I70" s="9"/>
@@ -4554,16 +4524,16 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="40">
-        <v>44713</v>
+        <v>44805</v>
       </c>
       <c r="B71" s="20" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C71" s="13">
         <v>1.25</v>
       </c>
       <c r="D71" s="39">
-        <v>10</v>
+        <v>0.49199999999999999</v>
       </c>
       <c r="E71" s="9"/>
       <c r="F71" s="20"/>
@@ -4574,42 +4544,44 @@
       <c r="H71" s="39"/>
       <c r="I71" s="9"/>
       <c r="J71" s="11"/>
-      <c r="K71" s="20" t="s">
-        <v>111</v>
-      </c>
+      <c r="K71" s="20"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" s="40"/>
+      <c r="A72" s="40">
+        <v>44835</v>
+      </c>
       <c r="B72" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="C72" s="13"/>
+        <v>101</v>
+      </c>
+      <c r="C72" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D72" s="39">
-        <v>0.44800000000000001</v>
+        <v>0.129</v>
       </c>
       <c r="E72" s="9"/>
       <c r="F72" s="20"/>
-      <c r="G72" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G72" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H72" s="39"/>
       <c r="I72" s="9"/>
       <c r="J72" s="11"/>
-      <c r="K72" s="20"/>
+      <c r="K72" s="49"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="40">
-        <v>44743</v>
+        <v>44866</v>
       </c>
       <c r="B73" s="20" t="s">
-        <v>109</v>
+        <v>72</v>
       </c>
       <c r="C73" s="13">
         <v>1.25</v>
       </c>
       <c r="D73" s="39">
-        <v>0.21000000000000002</v>
+        <v>5</v>
       </c>
       <c r="E73" s="9"/>
       <c r="F73" s="20"/>
@@ -4620,20 +4592,22 @@
       <c r="H73" s="39"/>
       <c r="I73" s="9"/>
       <c r="J73" s="11"/>
-      <c r="K73" s="20"/>
+      <c r="K73" s="20" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="40">
-        <v>44774</v>
+        <v>44896</v>
       </c>
       <c r="B74" s="20" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C74" s="13">
         <v>1.25</v>
       </c>
       <c r="D74" s="39">
-        <v>4</v>
+        <v>0.67100000000000004</v>
       </c>
       <c r="E74" s="9"/>
       <c r="F74" s="20"/>
@@ -4644,19 +4618,15 @@
       <c r="H74" s="39"/>
       <c r="I74" s="9"/>
       <c r="J74" s="11"/>
-      <c r="K74" s="20" t="s">
-        <v>107</v>
-      </c>
+      <c r="K74" s="20"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A75" s="40"/>
-      <c r="B75" s="20" t="s">
-        <v>108</v>
-      </c>
+      <c r="A75" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="B75" s="20"/>
       <c r="C75" s="13"/>
-      <c r="D75" s="39">
-        <v>9.8000000000000004E-2</v>
-      </c>
+      <c r="D75" s="39"/>
       <c r="E75" s="9"/>
       <c r="F75" s="20"/>
       <c r="G75" s="13" t="str">
@@ -4670,17 +4640,13 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="40">
-        <v>44805</v>
-      </c>
-      <c r="B76" s="20" t="s">
-        <v>105</v>
-      </c>
+        <v>44957</v>
+      </c>
+      <c r="B76" s="20"/>
       <c r="C76" s="13">
         <v>1.25</v>
       </c>
-      <c r="D76" s="39">
-        <v>0.49199999999999999</v>
-      </c>
+      <c r="D76" s="39"/>
       <c r="E76" s="9"/>
       <c r="F76" s="20"/>
       <c r="G76" s="13">
@@ -4694,17 +4660,13 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="40">
-        <v>44835</v>
-      </c>
-      <c r="B77" s="20" t="s">
-        <v>103</v>
-      </c>
+        <v>44985</v>
+      </c>
+      <c r="B77" s="20"/>
       <c r="C77" s="13">
         <v>1.25</v>
       </c>
-      <c r="D77" s="39">
-        <v>1</v>
-      </c>
+      <c r="D77" s="39"/>
       <c r="E77" s="9"/>
       <c r="F77" s="20"/>
       <c r="G77" s="13">
@@ -4714,43 +4676,37 @@
       <c r="H77" s="39"/>
       <c r="I77" s="9"/>
       <c r="J77" s="11"/>
-      <c r="K77" s="49">
-        <v>44848</v>
-      </c>
+      <c r="K77" s="20"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A78" s="40"/>
-      <c r="B78" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="C78" s="13"/>
-      <c r="D78" s="39">
-        <v>0.129</v>
-      </c>
+      <c r="A78" s="40">
+        <v>45016</v>
+      </c>
+      <c r="B78" s="20"/>
+      <c r="C78" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D78" s="39"/>
       <c r="E78" s="9"/>
       <c r="F78" s="20"/>
-      <c r="G78" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G78" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H78" s="39"/>
       <c r="I78" s="9"/>
       <c r="J78" s="11"/>
-      <c r="K78" s="49"/>
+      <c r="K78" s="20"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="40">
-        <v>44866</v>
-      </c>
-      <c r="B79" s="20" t="s">
-        <v>72</v>
-      </c>
+        <v>45046</v>
+      </c>
+      <c r="B79" s="20"/>
       <c r="C79" s="13">
         <v>1.25</v>
       </c>
-      <c r="D79" s="39">
-        <v>5</v>
-      </c>
+      <c r="D79" s="39"/>
       <c r="E79" s="9"/>
       <c r="F79" s="20"/>
       <c r="G79" s="13">
@@ -4760,45 +4716,37 @@
       <c r="H79" s="39"/>
       <c r="I79" s="9"/>
       <c r="J79" s="11"/>
-      <c r="K79" s="20" t="s">
-        <v>78</v>
-      </c>
+      <c r="K79" s="20"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A80" s="40"/>
-      <c r="B80" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="C80" s="13"/>
-      <c r="D80" s="39">
-        <v>3</v>
-      </c>
+      <c r="A80" s="40">
+        <v>45077</v>
+      </c>
+      <c r="B80" s="20"/>
+      <c r="C80" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D80" s="39"/>
       <c r="E80" s="9"/>
       <c r="F80" s="20"/>
-      <c r="G80" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G80" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H80" s="39"/>
       <c r="I80" s="9"/>
       <c r="J80" s="11"/>
-      <c r="K80" s="20" t="s">
-        <v>102</v>
-      </c>
+      <c r="K80" s="20"/>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="40">
-        <v>44896</v>
-      </c>
-      <c r="B81" s="20" t="s">
-        <v>100</v>
-      </c>
+        <v>45107</v>
+      </c>
+      <c r="B81" s="20"/>
       <c r="C81" s="13">
         <v>1.25</v>
       </c>
-      <c r="D81" s="39">
-        <v>0.67100000000000004</v>
-      </c>
+      <c r="D81" s="39"/>
       <c r="E81" s="9"/>
       <c r="F81" s="20"/>
       <c r="G81" s="13">
@@ -4811,17 +4759,19 @@
       <c r="K81" s="20"/>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A82" s="48" t="s">
-        <v>79</v>
+      <c r="A82" s="40">
+        <v>45138</v>
       </c>
       <c r="B82" s="20"/>
-      <c r="C82" s="13"/>
+      <c r="C82" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D82" s="39"/>
       <c r="E82" s="9"/>
       <c r="F82" s="20"/>
-      <c r="G82" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G82" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H82" s="39"/>
       <c r="I82" s="9"/>
@@ -4830,7 +4780,7 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="40">
-        <v>44957</v>
+        <v>45169</v>
       </c>
       <c r="B83" s="20"/>
       <c r="C83" s="13">
@@ -4850,7 +4800,7 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="40">
-        <v>44985</v>
+        <v>45199</v>
       </c>
       <c r="B84" s="20"/>
       <c r="C84" s="13">
@@ -4870,9 +4820,11 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="40">
-        <v>45016</v>
-      </c>
-      <c r="B85" s="20"/>
+        <v>45230</v>
+      </c>
+      <c r="B85" s="20" t="s">
+        <v>56</v>
+      </c>
       <c r="C85" s="13">
         <v>1.25</v>
       </c>
@@ -4883,16 +4835,22 @@
         <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
-      <c r="H85" s="39"/>
+      <c r="H85" s="39">
+        <v>2</v>
+      </c>
       <c r="I85" s="9"/>
       <c r="J85" s="11"/>
-      <c r="K85" s="20"/>
+      <c r="K85" s="20" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="40">
-        <v>45046</v>
-      </c>
-      <c r="B86" s="20"/>
+        <v>45260</v>
+      </c>
+      <c r="B86" s="20" t="s">
+        <v>56</v>
+      </c>
       <c r="C86" s="13">
         <v>1.25</v>
       </c>
@@ -4903,20 +4861,28 @@
         <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
-      <c r="H86" s="39"/>
+      <c r="H86" s="39">
+        <v>2</v>
+      </c>
       <c r="I86" s="9"/>
       <c r="J86" s="11"/>
-      <c r="K86" s="20"/>
+      <c r="K86" s="20" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="40">
-        <v>45077</v>
-      </c>
-      <c r="B87" s="20"/>
+        <v>45291</v>
+      </c>
+      <c r="B87" s="20" t="s">
+        <v>98</v>
+      </c>
       <c r="C87" s="13">
         <v>1.25</v>
       </c>
-      <c r="D87" s="39"/>
+      <c r="D87" s="39">
+        <v>7</v>
+      </c>
       <c r="E87" s="9"/>
       <c r="F87" s="20"/>
       <c r="G87" s="13">
@@ -4926,42 +4892,41 @@
       <c r="H87" s="39"/>
       <c r="I87" s="9"/>
       <c r="J87" s="11"/>
-      <c r="K87" s="20"/>
+      <c r="K87" s="20" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A88" s="40">
-        <v>45107</v>
-      </c>
-      <c r="B88" s="20"/>
-      <c r="C88" s="13">
-        <v>1.25</v>
-      </c>
-      <c r="D88" s="39"/>
+      <c r="A88" s="40"/>
+      <c r="B88" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C88" s="13"/>
+      <c r="D88" s="39">
+        <v>5</v>
+      </c>
       <c r="E88" s="9"/>
       <c r="F88" s="20"/>
-      <c r="G88" s="13">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v>1.25</v>
-      </c>
+      <c r="G88" s="13"/>
       <c r="H88" s="39"/>
       <c r="I88" s="9"/>
       <c r="J88" s="11"/>
-      <c r="K88" s="20"/>
+      <c r="K88" s="20" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A89" s="40">
-        <v>45138</v>
+      <c r="A89" s="48" t="s">
+        <v>96</v>
       </c>
       <c r="B89" s="20"/>
-      <c r="C89" s="13">
-        <v>1.25</v>
-      </c>
+      <c r="C89" s="13"/>
       <c r="D89" s="39"/>
       <c r="E89" s="9"/>
       <c r="F89" s="20"/>
-      <c r="G89" s="13">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v>1.25</v>
+      <c r="G89" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
       </c>
       <c r="H89" s="39"/>
       <c r="I89" s="9"/>
@@ -4970,38 +4935,40 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="40">
-        <v>45169</v>
-      </c>
-      <c r="B90" s="20"/>
-      <c r="C90" s="13">
-        <v>1.25</v>
-      </c>
+        <v>45322</v>
+      </c>
+      <c r="B90" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C90" s="13"/>
       <c r="D90" s="39"/>
       <c r="E90" s="9"/>
       <c r="F90" s="20"/>
-      <c r="G90" s="13">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v>1.25</v>
-      </c>
-      <c r="H90" s="39"/>
+      <c r="G90" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H90" s="39">
+        <v>2</v>
+      </c>
       <c r="I90" s="9"/>
       <c r="J90" s="11"/>
-      <c r="K90" s="20"/>
+      <c r="K90" s="20" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="40">
-        <v>45199</v>
+        <v>45351</v>
       </c>
       <c r="B91" s="20"/>
-      <c r="C91" s="13">
-        <v>1.25</v>
-      </c>
+      <c r="C91" s="13"/>
       <c r="D91" s="39"/>
       <c r="E91" s="9"/>
       <c r="F91" s="20"/>
-      <c r="G91" s="13">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v>1.25</v>
+      <c r="G91" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
       </c>
       <c r="H91" s="39"/>
       <c r="I91" s="9"/>
@@ -5009,106 +4976,71 @@
       <c r="K91" s="20"/>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A92" s="40">
-        <v>45230</v>
-      </c>
-      <c r="B92" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C92" s="13">
-        <v>1.25</v>
-      </c>
+      <c r="A92" s="40"/>
+      <c r="B92" s="20"/>
+      <c r="C92" s="13"/>
       <c r="D92" s="39"/>
       <c r="E92" s="9"/>
       <c r="F92" s="20"/>
-      <c r="G92" s="13">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v>1.25</v>
-      </c>
-      <c r="H92" s="39">
-        <v>2</v>
-      </c>
+      <c r="G92" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H92" s="39"/>
       <c r="I92" s="9"/>
       <c r="J92" s="11"/>
-      <c r="K92" s="20" t="s">
-        <v>95</v>
-      </c>
+      <c r="K92" s="20"/>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A93" s="40">
-        <v>45260</v>
-      </c>
-      <c r="B93" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C93" s="13">
-        <v>1.25</v>
-      </c>
+      <c r="A93" s="40"/>
+      <c r="B93" s="20"/>
+      <c r="C93" s="13"/>
       <c r="D93" s="39"/>
       <c r="E93" s="9"/>
       <c r="F93" s="20"/>
-      <c r="G93" s="13">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v>1.25</v>
-      </c>
-      <c r="H93" s="39">
-        <v>2</v>
-      </c>
+      <c r="G93" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H93" s="39"/>
       <c r="I93" s="9"/>
       <c r="J93" s="11"/>
-      <c r="K93" s="20" t="s">
-        <v>97</v>
-      </c>
+      <c r="K93" s="20"/>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A94" s="40">
-        <v>45291</v>
-      </c>
-      <c r="B94" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="C94" s="13">
-        <v>1.25</v>
-      </c>
-      <c r="D94" s="39">
-        <v>7</v>
-      </c>
+      <c r="A94" s="40"/>
+      <c r="B94" s="20"/>
+      <c r="C94" s="13"/>
+      <c r="D94" s="39"/>
       <c r="E94" s="9"/>
       <c r="F94" s="20"/>
-      <c r="G94" s="13">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v>1.25</v>
+      <c r="G94" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
       </c>
       <c r="H94" s="39"/>
       <c r="I94" s="9"/>
       <c r="J94" s="11"/>
-      <c r="K94" s="20" t="s">
-        <v>99</v>
-      </c>
+      <c r="K94" s="20"/>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="40"/>
-      <c r="B95" s="20" t="s">
-        <v>72</v>
-      </c>
+      <c r="B95" s="20"/>
       <c r="C95" s="13"/>
-      <c r="D95" s="39">
-        <v>5</v>
-      </c>
+      <c r="D95" s="39"/>
       <c r="E95" s="9"/>
       <c r="F95" s="20"/>
-      <c r="G95" s="13"/>
+      <c r="G95" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
       <c r="H95" s="39"/>
       <c r="I95" s="9"/>
       <c r="J95" s="11"/>
-      <c r="K95" s="20" t="s">
-        <v>121</v>
-      </c>
+      <c r="K95" s="20"/>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A96" s="48" t="s">
-        <v>96</v>
-      </c>
+      <c r="A96" s="40"/>
       <c r="B96" s="20"/>
       <c r="C96" s="13"/>
       <c r="D96" s="39"/>
@@ -5124,12 +5056,8 @@
       <c r="K96" s="20"/>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A97" s="40">
-        <v>45322</v>
-      </c>
-      <c r="B97" s="20" t="s">
-        <v>56</v>
-      </c>
+      <c r="A97" s="40"/>
+      <c r="B97" s="20"/>
       <c r="C97" s="13"/>
       <c r="D97" s="39"/>
       <c r="E97" s="9"/>
@@ -5138,19 +5066,13 @@
         <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H97" s="39">
-        <v>2</v>
-      </c>
+      <c r="H97" s="39"/>
       <c r="I97" s="9"/>
       <c r="J97" s="11"/>
-      <c r="K97" s="20" t="s">
-        <v>122</v>
-      </c>
+      <c r="K97" s="20"/>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A98" s="40">
-        <v>45351</v>
-      </c>
+      <c r="A98" s="40"/>
       <c r="B98" s="20"/>
       <c r="C98" s="13"/>
       <c r="D98" s="39"/>
@@ -5582,146 +5504,34 @@
       <c r="K124" s="20"/>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A125" s="40"/>
-      <c r="B125" s="20"/>
-      <c r="C125" s="13"/>
-      <c r="D125" s="39"/>
+      <c r="A125" s="41"/>
+      <c r="B125" s="15"/>
+      <c r="C125" s="42"/>
+      <c r="D125" s="43"/>
       <c r="E125" s="9"/>
-      <c r="F125" s="20"/>
-      <c r="G125" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H125" s="39"/>
+      <c r="F125" s="15"/>
+      <c r="G125" s="42" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H125" s="43"/>
       <c r="I125" s="9"/>
-      <c r="J125" s="11"/>
-      <c r="K125" s="20"/>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A126" s="40"/>
-      <c r="B126" s="20"/>
-      <c r="C126" s="13"/>
-      <c r="D126" s="39"/>
-      <c r="E126" s="9"/>
-      <c r="F126" s="20"/>
-      <c r="G126" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H126" s="39"/>
-      <c r="I126" s="9"/>
-      <c r="J126" s="11"/>
-      <c r="K126" s="20"/>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A127" s="40"/>
-      <c r="B127" s="20"/>
-      <c r="C127" s="13"/>
-      <c r="D127" s="39"/>
-      <c r="E127" s="9"/>
-      <c r="F127" s="20"/>
-      <c r="G127" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H127" s="39"/>
-      <c r="I127" s="9"/>
-      <c r="J127" s="11"/>
-      <c r="K127" s="20"/>
-    </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A128" s="40"/>
-      <c r="B128" s="20"/>
-      <c r="C128" s="13"/>
-      <c r="D128" s="39"/>
-      <c r="E128" s="9"/>
-      <c r="F128" s="20"/>
-      <c r="G128" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H128" s="39"/>
-      <c r="I128" s="9"/>
-      <c r="J128" s="11"/>
-      <c r="K128" s="20"/>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A129" s="40"/>
-      <c r="B129" s="20"/>
-      <c r="C129" s="13"/>
-      <c r="D129" s="39"/>
-      <c r="E129" s="9"/>
-      <c r="F129" s="20"/>
-      <c r="G129" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H129" s="39"/>
-      <c r="I129" s="9"/>
-      <c r="J129" s="11"/>
-      <c r="K129" s="20"/>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A130" s="40"/>
-      <c r="B130" s="20"/>
-      <c r="C130" s="13"/>
-      <c r="D130" s="39"/>
-      <c r="E130" s="9"/>
-      <c r="F130" s="20"/>
-      <c r="G130" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H130" s="39"/>
-      <c r="I130" s="9"/>
-      <c r="J130" s="11"/>
-      <c r="K130" s="20"/>
-    </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A131" s="40"/>
-      <c r="B131" s="20"/>
-      <c r="C131" s="13"/>
-      <c r="D131" s="39"/>
-      <c r="E131" s="9"/>
-      <c r="F131" s="20"/>
-      <c r="G131" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H131" s="39"/>
-      <c r="I131" s="9"/>
-      <c r="J131" s="11"/>
-      <c r="K131" s="20"/>
-    </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A132" s="41"/>
-      <c r="B132" s="15"/>
-      <c r="C132" s="42"/>
-      <c r="D132" s="43"/>
-      <c r="E132" s="9"/>
-      <c r="F132" s="15"/>
-      <c r="G132" s="42" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H132" s="43"/>
-      <c r="I132" s="9"/>
-      <c r="J132" s="12"/>
-      <c r="K132" s="15"/>
+      <c r="J125" s="12"/>
+      <c r="K125" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
@@ -5789,14 +5599,14 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="53"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -5807,16 +5617,16 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="55">
+      <c r="F3" s="54">
         <v>43101</v>
       </c>
-      <c r="G3" s="51"/>
+      <c r="G3" s="52"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="57"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="56"/>
     </row>
     <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
@@ -5829,16 +5639,16 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="51"/>
+      <c r="G4" s="52"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="53"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
@@ -5864,18 +5674,18 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53" t="s">
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
       <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">

</xml_diff>